<commit_message>
update with 2019 tile data
</commit_message>
<xml_diff>
--- a/Oyster/Spat/data/development/entry/2019/tile_spat_count_entry_jan2019.xlsx
+++ b/Oyster/Spat/data/development/entry/2019/tile_spat_count_entry_jan2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UF\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevenbeck\Desktop\Reef_Project\Git\Beck_LC_R\oyster\spat\data\development\entry\2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -995,7 +995,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="A2" sqref="A2:P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,8 +1054,12 @@
       <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43497</v>
+      </c>
       <c r="D2" s="1">
         <v>43525</v>
       </c>
@@ -1100,8 +1104,12 @@
       <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43497</v>
+      </c>
       <c r="D3" s="1">
         <v>43525</v>
       </c>
@@ -1146,8 +1154,12 @@
       <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43497</v>
+      </c>
       <c r="D4" s="1">
         <v>43525</v>
       </c>
@@ -1192,8 +1204,12 @@
       <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43497</v>
+      </c>
       <c r="D5" s="1">
         <v>43525</v>
       </c>
@@ -1238,8 +1254,12 @@
       <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43497</v>
+      </c>
       <c r="D6" s="1">
         <v>43525</v>
       </c>
@@ -1284,8 +1304,12 @@
       <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43497</v>
+      </c>
       <c r="D7" s="1">
         <v>43525</v>
       </c>
@@ -1330,8 +1354,12 @@
       <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43497</v>
+      </c>
       <c r="D8" s="1">
         <v>43525</v>
       </c>
@@ -1376,8 +1404,12 @@
       <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43497</v>
+      </c>
       <c r="D9" s="1">
         <v>43525</v>
       </c>
@@ -1422,8 +1454,12 @@
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43497</v>
+      </c>
       <c r="D10" s="1">
         <v>43525</v>
       </c>
@@ -1468,8 +1504,12 @@
       <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43497</v>
+      </c>
       <c r="D11" s="1">
         <v>43525</v>
       </c>
@@ -1514,8 +1554,12 @@
       <c r="A12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43497</v>
+      </c>
       <c r="D12" s="1">
         <v>43525</v>
       </c>
@@ -1560,8 +1604,12 @@
       <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43497</v>
+      </c>
       <c r="D13" s="1">
         <v>43525</v>
       </c>
@@ -1606,8 +1654,12 @@
       <c r="A14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43497</v>
+      </c>
       <c r="D14" s="1">
         <v>43525</v>
       </c>
@@ -1652,8 +1704,12 @@
       <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43497</v>
+      </c>
       <c r="D15" s="1">
         <v>43525</v>
       </c>
@@ -1698,8 +1754,12 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43497</v>
+      </c>
       <c r="D16" s="1">
         <v>43525</v>
       </c>
@@ -1744,8 +1804,12 @@
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43497</v>
+      </c>
       <c r="D17" s="1">
         <v>43525</v>
       </c>
@@ -1790,8 +1854,12 @@
       <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43497</v>
+      </c>
       <c r="D18" s="1">
         <v>43525</v>
       </c>
@@ -1836,8 +1904,12 @@
       <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43497</v>
+      </c>
       <c r="D19" s="1">
         <v>43525</v>
       </c>
@@ -1882,8 +1954,12 @@
       <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43497</v>
+      </c>
       <c r="D20" s="1">
         <v>43525</v>
       </c>
@@ -1928,8 +2004,12 @@
       <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43497</v>
+      </c>
       <c r="D21" s="1">
         <v>43525</v>
       </c>
@@ -1974,8 +2054,12 @@
       <c r="A22" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43497</v>
+      </c>
       <c r="D22" s="1">
         <v>43525</v>
       </c>
@@ -2020,8 +2104,12 @@
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C23" s="1">
+        <v>43497</v>
+      </c>
       <c r="D23" s="1">
         <v>43525</v>
       </c>
@@ -2066,8 +2154,12 @@
       <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43497</v>
+      </c>
       <c r="D24" s="1">
         <v>43525</v>
       </c>
@@ -2112,8 +2204,12 @@
       <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="B25" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43497</v>
+      </c>
       <c r="D25" s="1">
         <v>43525</v>
       </c>
@@ -2158,8 +2254,12 @@
       <c r="A26" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43497</v>
+      </c>
       <c r="D26" s="1">
         <v>43525</v>
       </c>
@@ -2204,8 +2304,12 @@
       <c r="A27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43497</v>
+      </c>
       <c r="D27" s="1">
         <v>43525</v>
       </c>
@@ -2250,8 +2354,12 @@
       <c r="A28" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43497</v>
+      </c>
       <c r="D28" s="1">
         <v>43525</v>
       </c>

</xml_diff>